<commit_message>
Reorganize project structure and update Excel files. 1) Move Excel handlers to dedicated directories (gemini/ and o1pro/). 2) Update Excel files. 3) Add output with comparison results. 4) Update requirements.txt.
</commit_message>
<xml_diff>
--- a/file1.xlsx
+++ b/file1.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="SheetX_OnlyInFile1" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -480,4 +481,34 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="n">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
+        <f>A1 * 2</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>